<commit_message>
minor changes to sample data
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greenjod/Documents/1.Projects/1.MG_epidemiology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greenjod/Documents/GitHub/Familial-Myasthenia-Gravis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665C2CEF-A2A7-D549-9CF4-214E1D12E41A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F2771C-98CB-B746-92E2-B907589B5A2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19740" xr2:uid="{E5564C3C-0974-BF4D-A831-245212A04B63}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19760" xr2:uid="{E5564C3C-0974-BF4D-A831-245212A04B63}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="143">
   <si>
     <t>worst_status:</t>
   </si>
@@ -359,151 +359,112 @@
     <t>histology_of_thymus_if_known</t>
   </si>
   <si>
-    <t>p1</t>
-  </si>
-  <si>
-    <t>p2</t>
-  </si>
-  <si>
-    <t>p3</t>
-  </si>
-  <si>
-    <t>p4</t>
-  </si>
-  <si>
-    <t>p5</t>
-  </si>
-  <si>
-    <t>p6</t>
-  </si>
-  <si>
-    <t>p7</t>
-  </si>
-  <si>
-    <t>p8</t>
-  </si>
-  <si>
-    <t>p9</t>
-  </si>
-  <si>
-    <t>p10</t>
-  </si>
-  <si>
-    <t>p11</t>
-  </si>
-  <si>
-    <t>p12</t>
-  </si>
-  <si>
-    <t>p13</t>
-  </si>
-  <si>
-    <t>p14</t>
-  </si>
-  <si>
-    <t>p15</t>
-  </si>
-  <si>
-    <t>p16</t>
-  </si>
-  <si>
-    <t>p17</t>
-  </si>
-  <si>
-    <t>p18</t>
-  </si>
-  <si>
-    <t>p19</t>
-  </si>
-  <si>
-    <t>p20</t>
-  </si>
-  <si>
-    <t>p21</t>
-  </si>
-  <si>
-    <t>p22</t>
-  </si>
-  <si>
-    <t>p23</t>
-  </si>
-  <si>
-    <t>p24</t>
-  </si>
-  <si>
-    <t>p25</t>
-  </si>
-  <si>
-    <t>p26</t>
-  </si>
-  <si>
-    <t>p27</t>
-  </si>
-  <si>
-    <t>p28</t>
-  </si>
-  <si>
-    <t>p29</t>
-  </si>
-  <si>
-    <t>p30</t>
-  </si>
-  <si>
-    <t>p31</t>
-  </si>
-  <si>
-    <t>p32</t>
-  </si>
-  <si>
-    <t>p33</t>
-  </si>
-  <si>
-    <t>p34</t>
-  </si>
-  <si>
-    <t>p35</t>
-  </si>
-  <si>
-    <t>p36</t>
-  </si>
-  <si>
-    <t>p37</t>
-  </si>
-  <si>
-    <t>p38</t>
-  </si>
-  <si>
-    <t>p39</t>
-  </si>
-  <si>
-    <t>p40</t>
-  </si>
-  <si>
-    <t>p41</t>
-  </si>
-  <si>
-    <t>p42</t>
-  </si>
-  <si>
-    <t>p43</t>
-  </si>
-  <si>
-    <t>p44</t>
-  </si>
-  <si>
-    <t>p45</t>
-  </si>
-  <si>
-    <t>p46</t>
-  </si>
-  <si>
-    <t>p47</t>
-  </si>
-  <si>
-    <t>p48</t>
-  </si>
-  <si>
-    <t>p49</t>
+    <t>du029</t>
+  </si>
+  <si>
+    <t>du032</t>
+  </si>
+  <si>
+    <t>du033</t>
+  </si>
+  <si>
+    <t>du036</t>
+  </si>
+  <si>
+    <t>du037</t>
+  </si>
+  <si>
+    <t>du038</t>
+  </si>
+  <si>
+    <t>du041</t>
+  </si>
+  <si>
+    <t>du042</t>
+  </si>
+  <si>
+    <t>du045</t>
+  </si>
+  <si>
+    <t>du046</t>
+  </si>
+  <si>
+    <t>du047</t>
+  </si>
+  <si>
+    <t>du048</t>
+  </si>
+  <si>
+    <t>du049</t>
+  </si>
+  <si>
+    <t>du051</t>
+  </si>
+  <si>
+    <t>du052</t>
+  </si>
+  <si>
+    <t>du054</t>
+  </si>
+  <si>
+    <t>du055</t>
+  </si>
+  <si>
+    <t>du057</t>
+  </si>
+  <si>
+    <t>iu-29</t>
+  </si>
+  <si>
+    <t>iu-31</t>
+  </si>
+  <si>
+    <t>iu-33</t>
+  </si>
+  <si>
+    <t>iu-34</t>
+  </si>
+  <si>
+    <t>iu-35</t>
+  </si>
+  <si>
+    <t>iu-38</t>
+  </si>
+  <si>
+    <t>iu-39</t>
+  </si>
+  <si>
+    <t>iu-40</t>
+  </si>
+  <si>
+    <t>iu-41</t>
+  </si>
+  <si>
+    <t>iu-42</t>
+  </si>
+  <si>
+    <t>iu-45</t>
+  </si>
+  <si>
+    <t>iu-47</t>
+  </si>
+  <si>
+    <t>iu-48</t>
+  </si>
+  <si>
+    <t>iu-49</t>
+  </si>
+  <si>
+    <t>iu-50</t>
+  </si>
+  <si>
+    <t>iu-55</t>
+  </si>
+  <si>
+    <t>iu-56</t>
+  </si>
+  <si>
+    <t>iu-57</t>
   </si>
 </sst>
 </file>
@@ -873,7 +834,7 @@
   <dimension ref="A1:BY50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="171" zoomScaleNormal="171" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9507,10 +9468,10 @@
     </row>
     <row r="38" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
@@ -9740,10 +9701,10 @@
     </row>
     <row r="39" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B39" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -9973,10 +9934,10 @@
     </row>
     <row r="40" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="C40" t="s">
         <v>17</v>
@@ -10206,10 +10167,10 @@
     </row>
     <row r="41" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="B41" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="C41" t="s">
         <v>17</v>
@@ -10439,10 +10400,10 @@
     </row>
     <row r="42" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B42" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="C42" t="s">
         <v>17</v>
@@ -10672,10 +10633,10 @@
     </row>
     <row r="43" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
         <v>17</v>
@@ -10905,10 +10866,10 @@
     </row>
     <row r="44" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B44" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
@@ -11138,10 +11099,10 @@
     </row>
     <row r="45" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="C45" t="s">
         <v>17</v>
@@ -11371,10 +11332,10 @@
     </row>
     <row r="46" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="B46" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C46" t="s">
         <v>17</v>
@@ -11604,10 +11565,10 @@
     </row>
     <row r="47" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="B47" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="C47" t="s">
         <v>17</v>
@@ -11837,10 +11798,10 @@
     </row>
     <row r="48" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="C48" t="s">
         <v>17</v>
@@ -12070,10 +12031,10 @@
     </row>
     <row r="49" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="B49" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
       <c r="C49" t="s">
         <v>17</v>
@@ -12303,10 +12264,10 @@
     </row>
     <row r="50" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="B50" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="C50" t="s">
         <v>17</v>

</xml_diff>